<commit_message>
recupération de toutes les information pour le projets et installation du connecteur pour la BD
</commit_message>
<xml_diff>
--- a/Exercice3/Produits_excel.xlsx
+++ b/Exercice3/Produits_excel.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C100"/>
+  <dimension ref="A1:C99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,12 +444,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>KICHOUSE Radiateurs Pour 2 Ensembles Gilet Thermique Ssd Accessoire De Refroidissement Pour Ordinateur Dissipateur De Chaleur D'entraînement D'état L'ordinateur Aluminium Composants étal</t>
+          <t>Dissipateur Thermique de Refroidisseur, Composants de Refroidissement Industriels de Dissipateur Thermique de Serveur SNK P48PS 2U pour CPU, Ordinateurs et Accessoires</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>9,49</t>
+          <t>19,49</t>
         </is>
       </c>
     </row>
@@ -464,7 +464,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>16,15</t>
+          <t>16,59</t>
         </is>
       </c>
     </row>
@@ -474,12 +474,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>osiuujkw Claviers sans cadre appareil clavier accessoires ordinateur composant pièces de rechange remplacement pour VivoBook S510</t>
+          <t>Dissipateur de Chaleur, SNK P0048PS 2U Serveur Dissipateur de Chaleur Refroidissement Industriel Dissipateurs de Chaleur en Aluminium Composants pour CPU Accessoires pour Ordinateur</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>16,09</t>
+          <t>19,53</t>
         </is>
       </c>
     </row>
@@ -519,12 +519,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>UGREEN Revodok 105 Hub USB C HDMI 4K PD 100W Charge 3 Data Ports Adaptateur Multiports Docking Station Compatible avec iPhone 16 15 Série MacBook iPad Pro Air 2024 Surface Galaxy S24 S23 Ultra</t>
+          <t>SanDisk 128 Go Extreme PRO carte SDXC + RescuePRO Deluxe, jusqu'à 200 Mo/s, UHS-I, Classe 10, U3, V30</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>15,99</t>
+          <t>21,25</t>
         </is>
       </c>
     </row>
@@ -534,12 +534,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>SanDisk 128 Go Extreme PRO carte SDXC + RescuePRO Deluxe, jusqu'à 200 Mo/s, UHS-I, Classe 10, U3, V30</t>
+          <t>UGREEN Câble USB C vers USB C PD Charge Rapide 60W Nylon Tressé Compatible avec iPhone 16 Plus Pro Max 15 Galaxy S24 Plus Ultra S23 A05S A35 A55 Redmi 14C A3 Note 13 iPad Pro Air MacBook Pro (1M）</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>20,95</t>
+          <t>6,97</t>
         </is>
       </c>
     </row>
@@ -549,12 +549,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Logitech M185 Souris Sans Fil, 2.4 GHz avec Mini Récepteur USB, Longévité de la Pile 12 Mois, Résolution du Capteur 1000 PPP, Ambidextre, Compatible PC, Mac, Ordinateur Portable - Gris/Noir</t>
+          <t>UGREEN Revodok 105 Hub USB C HDMI 4K PD 100W Charge 3 Data Ports Adaptateur Multiports Docking Station Compatible avec iPhone 16 15 Série MacBook iPad Pro Air 2024 Surface Galaxy S24 S23 Ultra</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>9,82</t>
+          <t>19,99</t>
         </is>
       </c>
     </row>
@@ -564,12 +564,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>UGREEN Câble USB C vers USB C PD Charge Rapide 60W Nylon Tressé Compatible avec iPhone 16 Plus Pro Max 15 Galaxy S24 Plus Ultra S23 A05S A35 A55 Redmi 14C A3 Note 13 iPad Pro Air MacBook Pro (1M）</t>
+          <t>Logitech M185 Souris Sans Fil, 2.4 GHz avec Mini Récepteur USB, Longévité de la Pile 12 Mois, Résolution du Capteur 1000 PPP, Ambidextre, Compatible PC, Mac, Ordinateur Portable - Gris/Noir</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>6,97</t>
+          <t>9,82</t>
         </is>
       </c>
     </row>
@@ -594,12 +594,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>UGREEN Adaptateur USB C vers A 3.2 10Gbps OTG Lot de 2 Compatible avec iPhone 16 Plus Pro Max 15 MacBook Air iMac iPad Galaxy Tab S9 S24 (Gris)</t>
+          <t>SanDisk 128 Go Ultra Dual Drive Go, Flash Drive Clé USB C, vitesse allant jusqu'à 400 Mo/s, Connecteurs USB Type-C et USB Type-A réversibles, Android smartphone stockage, Tablettes, Mac et PC, Noire</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>7,99</t>
+          <t>13,99</t>
         </is>
       </c>
     </row>
@@ -609,12 +609,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Zspeed Stylet ipad avec Chargement Sans Fil, iPad Pencil avec Rejet de Paume &amp; Sensibilité à l'inclinaison, Stylet pour iPad compatible avec iPad Pro 11/12.9, iPad 6/7/8/9/10, iPad Air/iPad Mini</t>
+          <t>UGREEN Adaptateur USB C vers A 3.2 10Gbps OTG Lot de 2 Compatible avec iPhone 16 Plus Pro Max 15 MacBook Air iMac iPad Galaxy Tab S9 S24 (Gris)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>18,99</t>
+          <t>9,99</t>
         </is>
       </c>
     </row>
@@ -629,7 +629,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>13,79</t>
+          <t>11,09</t>
         </is>
       </c>
     </row>
@@ -639,12 +639,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Gadpiparty 50 Pièces Accessoires informatiques Accessoires d'ordinateur Boîtier d'ordinateur Composants de PC vis longues du ventilateur de l'ordinateur vis métalliques pour ordinateur</t>
+          <t>osiuujkw Claviers sans cadre appareil clavier accessoires ordinateur composant pièces de rechange remplacement pour VivoBook S510</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>9,79</t>
+          <t>14,70</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>15,71</t>
+          <t>15,24</t>
         </is>
       </c>
     </row>
@@ -669,12 +669,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>SanDisk 128 Go Ultra Dual Drive Go, Flash Drive Clé USB C, vitesse allant jusqu'à 400 Mo/s, Connecteurs USB Type-C et USB Type-A réversibles, Android smartphone stockage, Tablettes, Mac et PC, Noire</t>
+          <t>SanDisk Extreme 128 Go microSDXC, Carte micro sd + adaptateur SD, UHS-I V30, jusqu'à 190 Mo/s, pour votre smartphone, caméra d'action ou droner, RescuePro Deluxe, A2, Class 10, U3</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>12,90</t>
+          <t>15,04</t>
         </is>
       </c>
     </row>
@@ -684,12 +684,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>SanDisk Extreme 128 Go microSDXC, Carte micro sd + adaptateur SD, UHS-I V30, jusqu'à 190 Mo/s, pour votre smartphone, caméra d'action ou droner, RescuePro Deluxe, A2, Class 10, U3</t>
+          <t>UGREEN Cat 8 Câble Ethernet Réseau RJ45 Super Débit 40Gbps 2000MHz Nylon Tressé Double Blindage Compatible avec Routeur Switch Modem Décodeur TV Box Internet PS5 PS4 Xbox Console de Jeux PC (1M)</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>13,99</t>
+          <t>6,99</t>
         </is>
       </c>
     </row>
@@ -699,12 +699,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>UGREEN Cat 8 Câble Ethernet Réseau RJ45 Super Débit 40Gbps 2000MHz Nylon Tressé Double Blindage Compatible avec Routeur Switch Modem Décodeur TV Box Internet PS5 PS4 Xbox Console de Jeux PC (1M)</t>
+          <t>TP-Link TL-SG105 Switch Ethernet Gigabit 5 ports RJ45 metallique 10/100/1000 Mbps, IGMP Snooping, switch RJ45 idéal pour étendre le réseau câblé pour les bureaux à domicile</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>6,99</t>
+          <t>15,73</t>
         </is>
       </c>
     </row>
@@ -714,12 +714,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>TP-Link TL-SG105 Switch Ethernet Gigabit 5 ports RJ45 metallique 10/100/1000 Mbps, IGMP Snooping, switch RJ45 idéal pour étendre le réseau câblé pour les bureaux à domicile</t>
+          <t>SanDisk 128 Go Ultra Flair Flash Drive Clé USB, des vitesses allant jusqu'à 150 Mo/s, USB 3.0, Protection par mot de passe, Un boîtier en métal élégant et resistant, Argent/Noir</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>15,73</t>
+          <t>12,29</t>
         </is>
       </c>
     </row>
@@ -734,7 +734,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>5,94</t>
+          <t>12,00</t>
         </is>
       </c>
     </row>
@@ -744,12 +744,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>SanDisk 128 Go Ultra Flair Flash Drive Clé USB, des vitesses allant jusqu'à 150 Mo/s, USB 3.0, Protection par mot de passe, Un boîtier en métal élégant et resistant, Argent/Noir</t>
+          <t>Kingston Technology Canvas Select Plus Carte MIcro SD SDCS2/128GB Class 10 + Adaptateur inclus</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>12,90</t>
+          <t>6,99</t>
         </is>
       </c>
     </row>
@@ -759,12 +759,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>ProCase 2 films de protection d'écran en verre trempé 9H pour iPad 10e génération 10,9" 2022 - Transparent</t>
+          <t>CSL-Computer - Tapis de souris XXL Speed Gaming Titanwolf noir 900 x 400 mm - Grande base de table - Améliore la précision et la vitesse, 23032532, Type 1</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>9,99</t>
+          <t>7,49</t>
         </is>
       </c>
     </row>
@@ -779,7 +779,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>12,78</t>
+          <t>12,95</t>
         </is>
       </c>
     </row>
@@ -789,12 +789,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>SanDisk 128 Go Extreme PRO microSDXC carte + adaptateur SD + RescuePro Deluxe jusqu'à 200 Mo/s avec des performances applicatives A2 UHS-I Class 10 U3 V30</t>
+          <t>ProCase 2 films de protection d'écran en verre trempé 9H pour iPad 10e génération 10,9" 2022 - Transparent</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>17,72</t>
+          <t>12,78</t>
         </is>
       </c>
     </row>
@@ -804,12 +804,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ilikable Lot de 3 Câble USB C vers Lightning 1M Cable iPhone Charge Rapide MFi Certifié Chargeur pour iPhone 14 13 12 Pro Max Mini iPhone 11 Pro X XR XS SE 2020 8 Plus</t>
+          <t>INIU Câble USB C vers USB C [100W/2M], Câble de Charge Rapide PD 5A QC 4.0, Câble Chargeur Nylon Tressé Type-C pour iPhone 16/15 Pro Max Samsung Galaxy S24/S23 A55/A35 iPad Air Mini MacBook Steam Deck</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>8,73</t>
+          <t>9,99</t>
         </is>
       </c>
     </row>
@@ -819,12 +819,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Lecteur CD DVD externe pour ordinateur portable USB 3.0 Type-C Portable Graveur DVD CD+/-RW Lecteur CD DVD externe pour PC, bureau, MacBook, iMac, Windows 11/10/8/7/XP/Vista/Linux/Mac/OS</t>
+          <t>SanDisk 128 Go Extreme PRO microSDXC carte + adaptateur SD + RescuePro Deluxe jusqu'à 200 Mo/s avec des performances applicatives A2 UHS-I Class 10 U3 V30</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>21,98</t>
+          <t>6,69</t>
         </is>
       </c>
     </row>
@@ -834,12 +834,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Kingston Technology Canvas Select Plus Carte MIcro SD SDCS2/128GB Class 10 + Adaptateur inclus</t>
+          <t>INIU Câble USB A vers USB C [Lot de 3 (2+2+0.5M)], Câble USB C 3.1A Charge Rapide, Câble de Charge USB-C Tressé en Nylon pour iPhone 16 15 Pro Max iPad Air Mini Samsung Galaxy S24 S23 S22 Ultra Xiaomi</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>7,49</t>
+          <t>17,95</t>
         </is>
       </c>
     </row>
@@ -849,12 +849,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>INIU Câble USB C vers USB C [100W/2M], Câble de Charge Rapide PD 5A QC 4.0, Câble Chargeur Nylon Tressé Type-C pour iPhone 16/15 Pro Max Samsung Galaxy S24/S23 A55/A35 iPad Air Mini MacBook Steam Deck</t>
+          <t>UGREEN Câble HDMI 4K Ultra HD Cordon 2.0 Haute Vitesse par Ethernet en Nylon Tressé Supporte 3D HDR Retour Audio Compatible avec PS5 PS4 PS3 Lecteur Blu Ray Xbox 360 PC Ampli TV Écran (2M)</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>6,15</t>
+          <t>9,99</t>
         </is>
       </c>
     </row>
@@ -864,12 +864,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>INIU Câble USB A vers USB C [Lot de 3 (2+2+0.5M)], Câble USB C 3.1A Charge Rapide, Câble de Charge USB-C Tressé en Nylon pour iPhone 16 15 Pro Max iPad Air Mini Samsung Galaxy S24 S23 S22 Ultra Xiaomi</t>
+          <t>ilikable Lot de 3 Câble USB C vers Lightning 1M Cable iPhone Charge Rapide MFi Certifié Chargeur pour iPhone 14 13 12 Pro Max Mini iPhone 11 Pro X XR XS SE 2020 8 Plus</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>9,98</t>
+          <t>8,59</t>
         </is>
       </c>
     </row>
@@ -879,12 +879,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>CSL-Computer - Tapis de souris XXL Speed Gaming Titanwolf noir 900 x 400 mm - Grande base de table - Améliore la précision et la vitesse, 23032532, Type 1</t>
+          <t>UGREEN USB 3.0 Lecteur de Carte SD Micro Adaptateur 5Gbps Transfert Rapide Accès Simultané à 2 Cartes Max 2To Card Reader Supporter TF SDXC SDHC MMC pour Windows MacOS Linux</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>12,95</t>
+          <t>11,89</t>
         </is>
       </c>
     </row>
@@ -899,7 +899,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>18,06</t>
+          <t>12,18</t>
         </is>
       </c>
     </row>
@@ -909,12 +909,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Denash Carte PCI Carte Graphique VGA 8 Mo 32 Bits Ordinateur de Bureau Composants Accessoires Multi-Affichage pour ATI Rage XL</t>
+          <t>Mikikit 1 Jeu Ordinateur M. 2 De Montage Composants De Montage Du Disque Dur Ssd Ssd Accessoire Informatique Pour M.2 Ssd Adaptateur Serveur Acier Inoxydable M2</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>19,42</t>
+          <t>17,28</t>
         </is>
       </c>
     </row>
@@ -929,7 +929,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>8,79</t>
+          <t>4,79</t>
         </is>
       </c>
     </row>
@@ -939,12 +939,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>KICHOUSE Radiateurs Pour 2 Ensembles Gilet Thermique Ssd Accessoire De Refroidissement Pour Ordinateur Dissipateur De Chaleur D'entraînement D'état L'ordinateur Aluminium Composants étal</t>
+          <t>Dissipateur Thermique de Refroidisseur, Composants de Refroidissement Industriels de Dissipateur Thermique de Serveur SNK P48PS 2U pour CPU, Ordinateurs et Accessoires</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>9,49</t>
+          <t>19,49</t>
         </is>
       </c>
     </row>
@@ -959,7 +959,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>16,15</t>
+          <t>16,59</t>
         </is>
       </c>
     </row>
@@ -969,12 +969,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>osiuujkw Claviers sans cadre appareil clavier accessoires ordinateur composant pièces de rechange remplacement pour VivoBook S510</t>
+          <t>Dissipateur de Chaleur, SNK P0048PS 2U Serveur Dissipateur de Chaleur Refroidissement Industriel Dissipateurs de Chaleur en Aluminium Composants pour CPU Accessoires pour Ordinateur</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>16,09</t>
+          <t>19,53</t>
         </is>
       </c>
     </row>
@@ -984,12 +984,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Lot de 4 adaptateurs USB C vers USB 3.0, adaptateur USB type C compatible avec iPhone 15, iPad, Samsung Galaxy S23 S22, MacBook, ChromeBook, Google Pixel</t>
+          <t>Lecteur Carte Identité Belge PC/SC USB Smart Card Reader, Support Digital Signature, Lecteur de Carte CAC,CRS,CNS,IC,SIM,Plug and Play,sans Pilote,Compatible Windows,Mac OS,Linux</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>6,29</t>
+          <t>16,88</t>
         </is>
       </c>
     </row>
@@ -999,12 +999,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>TP-Link Adaptateur Bluetooth 5.0 UB500, dongle bluetooth 5.0, clé bluetooth pour PC, casque, souris, manette, clavier, imprimantes, smartphone, tablette, compatible avec Windows 11/10/8.1/7</t>
+          <t>Arctic MX-4 Pasta Térmica 4 Gramos</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>8,79</t>
+          <t>6,90</t>
         </is>
       </c>
     </row>
@@ -1014,12 +1014,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>SanDisk SDSQUA4-032G-GN6MT, Lot de 2 cartes mémoire microSDXC Ultra 32 Go + Adaptateur SD. Vitesse de Lecture Allant jusqu'à 120Mo/S, Classe 10, U1, A1, rouge et gris</t>
+          <t>TP-Link Clé WiFi Puissante AC1300 Mbps, adaptateur USB wifi, dongle wifi, USB 3.0 Double Bande, 2.4G / 5GHz, MU-MIMO, compatible avec Windows 11/10/8.1/8/7/XP, Mac OS X, Archer T3U</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>9,94</t>
+          <t>15,99</t>
         </is>
       </c>
     </row>
@@ -1029,12 +1029,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>UGREEN Adaptateur USB A vers C 3.2 10Gbps Lot de 3 Convertisseur TypeC Femelle à TypeA Mâle Charge Rapide Data Sync Compatible avec iPhone 14 13 Plus Pro Max MacBook iPad Air Galaxy S24 A54</t>
+          <t>HP 305 Original Noir 1 pièce(s)</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>10,99</t>
+          <t>18,33</t>
         </is>
       </c>
     </row>
@@ -1044,12 +1044,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>UGREEN Câble HDMI 4K Ultra HD Cordon 2.0 Haute Vitesse par Ethernet en Nylon Tressé Supporte 3D HDR Retour Audio Compatible avec PS5 PS4 PS3 Lecteur Blu Ray Xbox 360 PC Ampli TV Écran (2M)</t>
+          <t>Kingston DataTraveler Exodia M Clé USB 3.2 Gen 1 DTXM/128GB - avec capuchon mobile (Noir + Rouge)</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>7,30</t>
+          <t>6,66</t>
         </is>
       </c>
     </row>
@@ -1059,12 +1059,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>UGREEN USB 3.0 Lecteur de Carte SD Micro Adaptateur 5Gbps Transfert Rapide Accès Simultané à 2 Cartes Max 2To Card Reader Supporter TF SDXC SDHC MMC pour Windows MacOS Linux</t>
+          <t>TP-Link Adaptateur Bluetooth 5.0 UB500, dongle bluetooth 5.0, clé bluetooth pour PC, casque, souris, manette, clavier, imprimantes, smartphone, tablette, compatible avec Windows 11/10/8.1/7</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>12,18</t>
+          <t>10,99</t>
         </is>
       </c>
     </row>
@@ -1074,12 +1074,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Samsung Pro Plus MB-MD256SA/EU Carte microSD + adaptateur SD 256 Go pour jeux mobiles sur smartphones, tablettes et consoles portables, UHS-I U3, Full HD &amp; 4K UHD, 180 Mo/s en lecture, 130 Mo/s en</t>
+          <t>UGREEN Adaptateur USB A vers C 3.2 10Gbps Lot de 3 Convertisseur TypeC Femelle à TypeA Mâle Charge Rapide Data Sync Compatible avec iPhone 14 13 Plus Pro Max MacBook iPad Air Galaxy S24 A54</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>18,04</t>
+          <t>5,99</t>
         </is>
       </c>
     </row>
@@ -1089,12 +1089,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>TP-Link Clé WiFi Puissante AC1300 Mbps, adaptateur USB wifi, dongle wifi, USB 3.0 Double Bande, 2.4G / 5GHz, MU-MIMO, compatible avec Windows 11/10/8.1/8/7/XP, Mac OS X, Archer T3U</t>
+          <t>MilnoTech Câble USB C 1M - Charge Rapide [Certifié MFi] pour iPhone 14/13/13PRO/12/12 PRO Max/12 Mini/11/11PRO/XS/XR/X/8/8Plus/iPad</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>15,99</t>
+          <t>18,00</t>
         </is>
       </c>
     </row>
@@ -1104,12 +1104,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Hub USB C, 6 en 1 DEMKICO Adaptateur Multiport Type C avec HDMI 4K, Lecteur de Cartes SD/TF, Port USB 3.0 &amp; USB 2.0, Port PD 100W, Compatible avec MacBook Pro/MacBook Air/Dell XPS et Plus Encore</t>
+          <t>Apple Câble USB-C vers Lightning (1 m) ​​​​​​​</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>14,99</t>
+          <t>9,33</t>
         </is>
       </c>
     </row>
@@ -1119,12 +1119,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Sniokco 10K 8K Câble HDMI 2.1 48Gbps 2M, Certifié Ultra Haute Vitesse HDMI® Cable 0.01ms 4K 240Hz 165Hz 120Hz 8K 60Hz eARC Netflix HDCP 2.3 2.2 DTS:X HDR10+ TV Moniteur Projecteur Roku PS5 X-box</t>
+          <t>SanDisk SDSQUA4-032G-GN6MT, Lot de 2 cartes mémoire microSDXC Ultra 32 Go + Adaptateur SD. Vitesse de Lecture Allant jusqu'à 120Mo/S, Classe 10, U1, A1, rouge et gris</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>10,79</t>
+          <t>19,44</t>
         </is>
       </c>
     </row>
@@ -1134,12 +1134,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Kingston Technology DataTraveler Exodia DTX/64GB Flash Drive USB 3.2 Gen 1 - avec capuchon de protection et porte-clés en couleurs multiples</t>
+          <t>Logitech C270 Webcam Streaming HD, 720p/30ips, Appel Vidéo HD Large Champ de Vision, Correction de la Lumière, Micro Antiparasites, Skype, FaceTime, Camera PC/Mac/Portable/Tablette/Chromebook</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>4,69</t>
+          <t>14,99</t>
         </is>
       </c>
     </row>
@@ -1149,12 +1149,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Kingston DataTraveler Exodia M Clé USB 3.2 Gen 1 DTXM/128GB - avec capuchon mobile (Noir + Rouge)</t>
+          <t>Hub USB C, 6 en 1 DEMKICO Adaptateur Multiport Type C avec HDMI 4K, Lecteur de Cartes SD/TF, Port USB 3.0 &amp; USB 2.0, Port PD 100W, Compatible avec MacBook Pro/MacBook Air/Dell XPS et Plus Encore</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>6,66</t>
+          <t>11,09</t>
         </is>
       </c>
     </row>
@@ -1169,7 +1169,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>13,79</t>
+          <t>14,70</t>
         </is>
       </c>
     </row>
@@ -1179,12 +1179,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Gadpiparty 50 Pièces Accessoires informatiques Accessoires d'ordinateur Boîtier d'ordinateur Composants de PC vis longues du ventilateur de l'ordinateur vis métalliques pour ordinateur</t>
+          <t>osiuujkw Claviers sans cadre appareil clavier accessoires ordinateur composant pièces de rechange remplacement pour VivoBook S510</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>9,79</t>
+          <t>15,24</t>
         </is>
       </c>
     </row>
@@ -1199,7 +1199,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>15,71</t>
+          <t>5,99</t>
         </is>
       </c>
     </row>
@@ -1209,12 +1209,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Metapen Stylet A8 pour Ipad, Précision au Pixel Près et Faible Latence de Pointe, Idéal pour Prendre des Notes, Dessiner et Signer, Apple Pencil avec Ipad 10/9/8/7/6, Pro 3/4/5/6, Air 3/4/5, Mini5/6</t>
+          <t>Lot de 4 adaptateurs USB C vers USB 3.0, adaptateur USB type C compatible avec iPhone 15, iPad, Samsung Galaxy S23 S22, MacBook, ChromeBook, Google Pixel</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>18,99</t>
+          <t>4,69</t>
         </is>
       </c>
     </row>
@@ -1224,12 +1224,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Razer DeathAdder Essential (2021) - Souris Gaming Filaire avec Capteur Optique de 6400 DPI (Design Ergonomique, 5 Boutons Programmables, Jusqu'à 10M de Clics) Noir</t>
+          <t>Kingston Technology DataTraveler Exodia DTX/64GB Flash Drive USB 3.2 Gen 1 - avec capuchon de protection et porte-clés en couleurs multiples</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>19,99</t>
+          <t>7,99</t>
         </is>
       </c>
     </row>
@@ -1239,12 +1239,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>KECOW Stylet pour ipad 2018-2024, ipad Pencil avec Adsorption Magnétique &amp; Rejet de Palme, Apple Pencil pour iPad Air M2/3/4/5, iPad Pro M4, iPad Pro 11" 4/3/2/1, iPad Pro 12,9" 3/4/5/6, iPad Mini 5/6</t>
+          <t>Arctic Mx-4 Highest Performance Thermal Compound, ACTCP00031B</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>15,19</t>
+          <t>19,99</t>
         </is>
       </c>
     </row>
@@ -1254,12 +1254,12 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Arctic MX-4 Pasta Térmica 4 Gramos</t>
+          <t>Razer DeathAdder Essential (2021) - Souris Gaming Filaire avec Capteur Optique de 6400 DPI (Design Ergonomique, 5 Boutons Programmables, Jusqu'à 10M de Clics) Noir</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>6,90</t>
+          <t>18,52</t>
         </is>
       </c>
     </row>
@@ -1269,12 +1269,12 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Vinmooog Souris sans fil Bluetooth rechargeable sans fil pour ordinateur portable, souris verticale rétroéclairée de 7 couleurs, 3 dpi Récepteur USB 2,4 GHz Ultra mince</t>
+          <t>ORIGBELIE Lecteur CD Externe USB 3.0 et Type-C Portable CD/DVD +/-RW Graveur DVD Externe, Ultra Mince Lecteur DVD Externe pour PC Laptop Desktop iMac MacBook Pro/Air Windows 11/10/8/7/XP Linux Mac OS</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>8,49</t>
+          <t>4,49</t>
         </is>
       </c>
     </row>
@@ -1284,12 +1284,12 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>UGREEN Lot de 2 Câble USB C vers USB C PD Charge Rapide 60W Nylon Tressé Compatible avec iPhone 16 Plus Pro Max 15 Galaxy S24 S23 A05S A35 A55 Redmi 14C A3 Note 13 12 MacBook Pro iPad Pro (1M)</t>
+          <t>Logitech M90 Souris Filaire USB, Suivi Optique 1000 PPP, Ambidextre, Compatible avec PC/Mac/Portable - Noir</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>10,99</t>
+          <t>5,98</t>
         </is>
       </c>
     </row>
@@ -1299,12 +1299,12 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Logitech C270 Webcam Streaming HD, 720p/30ips, Appel Vidéo HD Large Champ de Vision, Correction de la Lumière, Micro Antiparasites, Skype, FaceTime, Camera PC/Mac/Portable/Tablette/Chromebook</t>
+          <t>Adaptateur USB C vers USB (Lot de 4), Adaptateur USB-C Mâle vers USB-A 3.0 Femelle OTG Compatible avec MacBook Pro, Samsung Galaxy, Téléphones Type-C et Plus (Noir)</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>16,54</t>
+          <t>8,59</t>
         </is>
       </c>
     </row>
@@ -1314,12 +1314,12 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Aceele HUB USB 3.0 5 Ports (avec Alimentation), Ultra-Fin avec 4 Ports de Données USB 3.0, SuperSpeed 5Gbps, Micro USB Port D'alimentation, pour MacBook Air/Pro, Surface Pro, Dell XPS 15, Clé USB</t>
+          <t>Adaptateur USB C vers HDMI, HDMI vers USB C 4K Thunderbolt 3 vers HDMI, compatible avec iPhone 16/15Pro Max MacBook Pro/Air, Surface Pro, Pixelbook, iPad Pro, XPS, Samsung Galaxy S/Note Huawei Mate</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>8,99</t>
+          <t>12,99</t>
         </is>
       </c>
     </row>
@@ -1329,12 +1329,12 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>EooCoo Coque Compatible avec MacBook Air M2 M3 13.6 Pouces A2681 A3113, 2022 2024 Release avec Touch ID, Protection Coque Rigide en Plastique pour MacBook Air 13 M3 M2 - Transparent Clair</t>
+          <t>UGREEN Hub USB 3.0 4 Data Ports Ultra Fin Multiport Type A 5Gbps Haute Vitesse Compatible avec MacBook iMac Surface XPS PC Ordinateur Portable Disque Dur Clavier Souris (15cm)</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>14,98</t>
+          <t>9,95</t>
         </is>
       </c>
     </row>
@@ -1344,12 +1344,12 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Arctic Mx-4 Highest Performance Thermal Compound, ACTCP00031B</t>
+          <t>CLé USB 128 Go, 2 en 1 USB C Pendrive 128gb Portable Clef USB 128go Type C Memory Stick 128 GB pour Huawei Oneplus OTG Android Appareils TéLévision (Noir)</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>6,26</t>
+          <t>14,24</t>
         </is>
       </c>
     </row>
@@ -1359,12 +1359,12 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>UGREEN Hub USB 3.0 4 Data Ports Ultra Fin Multiport Type A 5Gbps Haute Vitesse Compatible avec MacBook iMac Surface XPS PC Ordinateur Portable Disque Dur Clavier Souris (15cm)</t>
+          <t>UGREEN Lot de 2 Câble USB C vers USB C PD 100W 5A 20V Charge Rapide Compatible avec MacBook iPad Pro iPhone 16 Plus Pro Max 15 Galaxy S24 Plus Ultra S23 A55 Steam Deck PS5 Manette (2M)</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>12,99</t>
+          <t>15,19</t>
         </is>
       </c>
     </row>
@@ -1374,12 +1374,12 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Trust Gaming GXT 415 Zirox Casque Gaming Léger avec Transducteurs 50 mm pour PC, Xbox, PS4, PS5, Switch, Mobile, Audio Jack 3.5 mm, Câble de 2 m, Casque Gamer Filaire Over-Ear avec Micro - Noir</t>
+          <t>KECOW Stylet pour ipad 2018-2024, ipad Pencil avec Adsorption Magnétique &amp; Rejet de Palme, Apple Pencil pour iPad Air M2/3/4/5, iPad Pro M4, iPad Pro 11" 4/3/2/1, iPad Pro 12,9" 3/4/5/6, iPad Mini 5/6</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>16,00</t>
+          <t>17,28</t>
         </is>
       </c>
     </row>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>18,06</t>
+          <t>4,79</t>
         </is>
       </c>
     </row>
@@ -1404,12 +1404,12 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Denash Carte PCI Carte Graphique VGA 8 Mo 32 Bits Ordinateur de Bureau Composants Accessoires Multi-Affichage pour ATI Rage XL</t>
+          <t>Mikikit 1 Jeu Ordinateur M. 2 De Montage Composants De Montage Du Disque Dur Ssd Ssd Accessoire Informatique Pour M.2 Ssd Adaptateur Serveur Acier Inoxydable M2</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>19,42</t>
+          <t>7,89</t>
         </is>
       </c>
     </row>
@@ -1419,12 +1419,12 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>UKCOCO Accessoires Pour Ordinateur Portable D'Ordinateur 1 Pièce Composant De Bandoulière Matériel De Sport Pour Hommes Et Femmes Bretelles Réglables</t>
+          <t>Dissipateur Thermique de Refroidisseur, Composants de Refroidissement Industriels de Dissipateur Thermique de Serveur SNK P48PS 2U pour CPU, Ordinateurs et Accessoires</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>8,79</t>
+          <t>19,49</t>
         </is>
       </c>
     </row>
@@ -1434,12 +1434,12 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>KICHOUSE Radiateurs Pour 2 Ensembles Gilet Thermique Ssd Accessoire De Refroidissement Pour Ordinateur Dissipateur De Chaleur D'entraînement D'état L'ordinateur Aluminium Composants étal</t>
+          <t>YWBL-WH Webcam USB2.0, USB2.0 avec caméra Web HD MIC 300 000 Pixels Cam 360 ° pour Ordinateur Portable PC pour Skype/MSN, Microphone intégré, Accessoires Et Pièces D'Ordinateur</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>9,49</t>
+          <t>16,59</t>
         </is>
       </c>
     </row>
@@ -1449,12 +1449,12 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>YWBL-WH Webcam USB2.0, USB2.0 avec caméra Web HD MIC 300 000 Pixels Cam 360 ° pour Ordinateur Portable PC pour Skype/MSN, Microphone intégré, Accessoires Et Pièces D'Ordinateur</t>
+          <t>Dissipateur de Chaleur, SNK P0048PS 2U Serveur Dissipateur de Chaleur Refroidissement Industriel Dissipateurs de Chaleur en Aluminium Composants pour CPU Accessoires pour Ordinateur</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>16,15</t>
+          <t>19,53</t>
         </is>
       </c>
     </row>
@@ -1464,12 +1464,12 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>osiuujkw Claviers sans cadre appareil clavier accessoires ordinateur composant pièces de rechange remplacement pour VivoBook S510</t>
+          <t>SanDisk 128 Go Ultra microSDXC, Carte micro sd + adaptateur SD (Pour Smartphone et Tablette, Video Full HDD, jusqu'à 140 Mo/s, UHS-I, La performance A1, Class 10, U1)</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>16,09</t>
+          <t>12,90</t>
         </is>
       </c>
     </row>
@@ -1479,12 +1479,12 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>SanDisk 128 Go Ultra microSDXC, Carte micro sd + adaptateur SD (Pour Smartphone et Tablette, Video Full HDD, jusqu'à 140 Mo/s, UHS-I, La performance A1, Class 10, U1)</t>
+          <t>Trust Lecteur DNI, Compatible avec Toutes Les Cartes DNI, Conforme FIPS 201, FIPS TAA et ISO 7816 Classe A, B, C, câble de 100 cm, USB Plug &amp; Play</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>12,90</t>
+          <t>9,99</t>
         </is>
       </c>
     </row>
@@ -1494,12 +1494,12 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Trust Lecteur DNI, Compatible avec Toutes Les Cartes DNI, Conforme FIPS 201, FIPS TAA et ISO 7816 Classe A, B, C, câble de 100 cm, USB Plug &amp; Play</t>
+          <t>SanDisk 128 Go Extreme PRO carte SDXC + RescuePRO Deluxe, jusqu'à 200 Mo/s, UHS-I, Classe 10, U3, V30</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>9,99</t>
+          <t>21,25</t>
         </is>
       </c>
     </row>
@@ -1509,12 +1509,12 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>UGREEN Revodok 105 Hub USB C HDMI 4K PD 100W Charge 3 Data Ports Adaptateur Multiports Docking Station Compatible avec iPhone 16 15 Série MacBook iPad Pro Air 2024 Surface Galaxy S24 S23 Ultra</t>
+          <t>UGREEN Câble USB C vers USB C PD Charge Rapide 60W Nylon Tressé Compatible avec iPhone 16 Plus Pro Max 15 Galaxy S24 Plus Ultra S23 A05S A35 A55 Redmi 14C A3 Note 13 iPad Pro Air MacBook Pro (1M）</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>15,99</t>
+          <t>6,97</t>
         </is>
       </c>
     </row>
@@ -1524,12 +1524,12 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>SanDisk 128 Go Extreme PRO carte SDXC + RescuePRO Deluxe, jusqu'à 200 Mo/s, UHS-I, Classe 10, U3, V30</t>
+          <t>UGREEN Revodok 105 Hub USB C HDMI 4K PD 100W Charge 3 Data Ports Adaptateur Multiports Docking Station Compatible avec iPhone 16 15 Série MacBook iPad Pro Air 2024 Surface Galaxy S24 S23 Ultra</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>20,95</t>
+          <t>19,99</t>
         </is>
       </c>
     </row>
@@ -1554,12 +1554,12 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>UGREEN Câble USB C vers USB C PD Charge Rapide 60W Nylon Tressé Compatible avec iPhone 16 Plus Pro Max 15 Galaxy S24 Plus Ultra S23 A05S A35 A55 Redmi 14C A3 Note 13 iPad Pro Air MacBook Pro (1M）</t>
+          <t>Quntis Lot de 3 Câble de Chargeur iPhone 2M, MFi Certifié Câble, Fil Lightning Charge Rapide pour iPhone 11 12 13 14 Pro 13 Mini XS Max XR X 8 7 6s 6 Plus 5 Se iPad Chargeur, Cordon iPhone Blanc</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>6,97</t>
+          <t>9,89</t>
         </is>
       </c>
     </row>
@@ -1569,12 +1569,12 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Quntis Lot de 3 Câble de Chargeur iPhone 2M, MFi Certifié Câble, Fil Lightning Charge Rapide pour iPhone 11 12 13 14 Pro 13 Mini XS Max XR X 8 7 6s 6 Plus 5 Se iPad Chargeur, Cordon iPhone Blanc</t>
+          <t>SanDisk 128 Go Ultra Dual Drive Go, Flash Drive Clé USB C, vitesse allant jusqu'à 400 Mo/s, Connecteurs USB Type-C et USB Type-A réversibles, Android smartphone stockage, Tablettes, Mac et PC, Noire</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>9,89</t>
+          <t>13,99</t>
         </is>
       </c>
     </row>
@@ -1589,7 +1589,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>7,99</t>
+          <t>9,99</t>
         </is>
       </c>
     </row>
@@ -1599,12 +1599,12 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Zspeed Stylet ipad avec Chargement Sans Fil, iPad Pencil avec Rejet de Paume &amp; Sensibilité à l'inclinaison, Stylet pour iPad compatible avec iPad Pro 11/12.9, iPad 6/7/8/9/10, iPad Air/iPad Mini</t>
+          <t>OSALADI 100 Pcs Accessoires Informatiques Vis De Montage Du Ventilateur Boîtier De L'Ordinateur Vis Du Ventilateur Ordinateur Ventilateur Vis Longue Composants Informatiques Ordinateur</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>18,99</t>
+          <t>11,09</t>
         </is>
       </c>
     </row>
@@ -1614,12 +1614,12 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>OSALADI 100 Pcs Accessoires Informatiques Vis De Montage Du Ventilateur Boîtier De L'Ordinateur Vis Du Ventilateur Ordinateur Ventilateur Vis Longue Composants Informatiques Ordinateur</t>
+          <t>osiuujkw Claviers sans cadre appareil clavier accessoires ordinateur composant pièces de rechange remplacement pour VivoBook S510</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>13,79</t>
+          <t>14,70</t>
         </is>
       </c>
     </row>
@@ -1629,12 +1629,12 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Gadpiparty 50 Pièces Accessoires informatiques Accessoires d'ordinateur Boîtier d'ordinateur Composants de PC vis longues du ventilateur de l'ordinateur vis métalliques pour ordinateur</t>
+          <t>Filtre pour Refroidissement à L'eau, Ordinateur G1 4 Filetage 4'' Électronique Intérieure Accessoires pour Ordinateur Composants Ventilateurs Intérieurs Systèmes de Refroidissement avec Large</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>9,79</t>
+          <t>15,24</t>
         </is>
       </c>
     </row>
@@ -1644,12 +1644,12 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Filtre pour Refroidissement à L'eau, Ordinateur G1 4 Filetage 4'' Électronique Intérieure Accessoires pour Ordinateur Composants Ventilateurs Intérieurs Systèmes de Refroidissement avec Large</t>
+          <t>SanDisk Extreme 128 Go microSDXC, Carte micro sd + adaptateur SD, UHS-I V30, jusqu'à 190 Mo/s, pour votre smartphone, caméra d'action ou droner, RescuePro Deluxe, A2, Class 10, U3</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>15,71</t>
+          <t>15,04</t>
         </is>
       </c>
     </row>
@@ -1659,12 +1659,12 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>SanDisk 128 Go Ultra Dual Drive Go, Flash Drive Clé USB C, vitesse allant jusqu'à 400 Mo/s, Connecteurs USB Type-C et USB Type-A réversibles, Android smartphone stockage, Tablettes, Mac et PC, Noire</t>
+          <t>UGREEN Cat 8 Câble Ethernet Réseau RJ45 Super Débit 40Gbps 2000MHz Nylon Tressé Double Blindage Compatible avec Routeur Switch Modem Décodeur TV Box Internet PS5 PS4 Xbox Console de Jeux PC (1M)</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>12,90</t>
+          <t>6,99</t>
         </is>
       </c>
     </row>
@@ -1674,12 +1674,12 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>SanDisk Extreme 128 Go microSDXC, Carte micro sd + adaptateur SD, UHS-I V30, jusqu'à 190 Mo/s, pour votre smartphone, caméra d'action ou droner, RescuePro Deluxe, A2, Class 10, U3</t>
+          <t>TP-Link TL-SG105 Switch Ethernet Gigabit 5 ports RJ45 metallique 10/100/1000 Mbps, IGMP Snooping, switch RJ45 idéal pour étendre le réseau câblé pour les bureaux à domicile</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>13,99</t>
+          <t>15,73</t>
         </is>
       </c>
     </row>
@@ -1689,12 +1689,12 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>UGREEN Cat 8 Câble Ethernet Réseau RJ45 Super Débit 40Gbps 2000MHz Nylon Tressé Double Blindage Compatible avec Routeur Switch Modem Décodeur TV Box Internet PS5 PS4 Xbox Console de Jeux PC (1M)</t>
+          <t>SanDisk 128 Go Ultra Flair Flash Drive Clé USB, des vitesses allant jusqu'à 150 Mo/s, USB 3.0, Protection par mot de passe, Un boîtier en métal élégant et resistant, Argent/Noir</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>6,99</t>
+          <t>12,29</t>
         </is>
       </c>
     </row>
@@ -1704,12 +1704,12 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>TP-Link TL-SG105 Switch Ethernet Gigabit 5 ports RJ45 metallique 10/100/1000 Mbps, IGMP Snooping, switch RJ45 idéal pour étendre le réseau câblé pour les bureaux à domicile</t>
+          <t>UGREEN Câble USB C Charge Rapide 3A Nylon Tressé Câble Chargeur USB C Compatible avec iPhone 16 Plus Pro Max 15 Galaxy S24 Plus Ultra S23 A05S A35 A55 Redmi 14C A3 Note 13 Manette PS5 (0.5M)</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>15,73</t>
+          <t>12,00</t>
         </is>
       </c>
     </row>
@@ -1719,12 +1719,12 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>UGREEN Câble USB C Charge Rapide 3A Nylon Tressé Câble Chargeur USB C Compatible avec iPhone 16 Plus Pro Max 15 Galaxy S24 Plus Ultra S23 A05S A35 A55 Redmi 14C A3 Note 13 Manette PS5 (0.5M)</t>
+          <t>Kingston Technology Canvas Select Plus Carte MIcro SD SDCS2/128GB Class 10 + Adaptateur inclus</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>5,94</t>
+          <t>6,99</t>
         </is>
       </c>
     </row>
@@ -1734,12 +1734,12 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>SanDisk 128 Go Ultra Flair Flash Drive Clé USB, des vitesses allant jusqu'à 150 Mo/s, USB 3.0, Protection par mot de passe, Un boîtier en métal élégant et resistant, Argent/Noir</t>
+          <t>CSL-Computer - Tapis de souris XXL Speed Gaming Titanwolf noir 900 x 400 mm - Grande base de table - Améliore la précision et la vitesse, 23032532, Type 1</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>12,90</t>
+          <t>7,49</t>
         </is>
       </c>
     </row>
@@ -1749,12 +1749,12 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>ProCase 2 films de protection d'écran en verre trempé 9H pour iPad 10e génération 10,9" 2022 - Transparent</t>
+          <t>AiTodos® Support Ordinateur Portable, Laptop Stand,Alliage D'aluminium, Léger, Compact Portable Pliable - Ventilation et Dissipation de la Chaleur, Réglage à 6 Vitesses - Support pc Portable</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>9,99</t>
+          <t>12,95</t>
         </is>
       </c>
     </row>
@@ -1764,7 +1764,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>AiTodos® Support Ordinateur Portable, Laptop Stand,Alliage D'aluminium, Léger, Compact Portable Pliable - Ventilation et Dissipation de la Chaleur, Réglage à 6 Vitesses - Support pc Portable</t>
+          <t>ProCase 2 films de protection d'écran en verre trempé 9H pour iPad 10e génération 10,9" 2022 - Transparent</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -1779,12 +1779,12 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>SanDisk 128 Go Extreme PRO microSDXC carte + adaptateur SD + RescuePro Deluxe jusqu'à 200 Mo/s avec des performances applicatives A2 UHS-I Class 10 U3 V30</t>
+          <t>INIU Câble USB C vers USB C [100W/2M], Câble de Charge Rapide PD 5A QC 4.0, Câble Chargeur Nylon Tressé Type-C pour iPhone 16/15 Pro Max Samsung Galaxy S24/S23 A55/A35 iPad Air Mini MacBook Steam Deck</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>17,72</t>
+          <t>9,99</t>
         </is>
       </c>
     </row>
@@ -1794,12 +1794,12 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>ilikable Lot de 3 Câble USB C vers Lightning 1M Cable iPhone Charge Rapide MFi Certifié Chargeur pour iPhone 14 13 12 Pro Max Mini iPhone 11 Pro X XR XS SE 2020 8 Plus</t>
+          <t>SanDisk 128 Go Extreme PRO microSDXC carte + adaptateur SD + RescuePro Deluxe jusqu'à 200 Mo/s avec des performances applicatives A2 UHS-I Class 10 U3 V30</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>8,73</t>
+          <t>6,69</t>
         </is>
       </c>
     </row>
@@ -1809,12 +1809,12 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Lecteur CD DVD externe pour ordinateur portable USB 3.0 Type-C Portable Graveur DVD CD+/-RW Lecteur CD DVD externe pour PC, bureau, MacBook, iMac, Windows 11/10/8/7/XP/Vista/Linux/Mac/OS</t>
+          <t>INIU Câble USB A vers USB C [Lot de 3 (2+2+0.5M)], Câble USB C 3.1A Charge Rapide, Câble de Charge USB-C Tressé en Nylon pour iPhone 16 15 Pro Max iPad Air Mini Samsung Galaxy S24 S23 S22 Ultra Xiaomi</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>21,98</t>
+          <t>17,95</t>
         </is>
       </c>
     </row>
@@ -1824,12 +1824,12 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Kingston Technology Canvas Select Plus Carte MIcro SD SDCS2/128GB Class 10 + Adaptateur inclus</t>
+          <t>UGREEN Câble HDMI 4K Ultra HD Cordon 2.0 Haute Vitesse par Ethernet en Nylon Tressé Supporte 3D HDR Retour Audio Compatible avec PS5 PS4 PS3 Lecteur Blu Ray Xbox 360 PC Ampli TV Écran (2M)</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>7,49</t>
+          <t>9,99</t>
         </is>
       </c>
     </row>
@@ -1839,12 +1839,12 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>INIU Câble USB C vers USB C [100W/2M], Câble de Charge Rapide PD 5A QC 4.0, Câble Chargeur Nylon Tressé Type-C pour iPhone 16/15 Pro Max Samsung Galaxy S24/S23 A55/A35 iPad Air Mini MacBook Steam Deck</t>
+          <t>ilikable Lot de 3 Câble USB C vers Lightning 1M Cable iPhone Charge Rapide MFi Certifié Chargeur pour iPhone 14 13 12 Pro Max Mini iPhone 11 Pro X XR XS SE 2020 8 Plus</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>6,15</t>
+          <t>8,59</t>
         </is>
       </c>
     </row>
@@ -1854,12 +1854,12 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>INIU Câble USB A vers USB C [Lot de 3 (2+2+0.5M)], Câble USB C 3.1A Charge Rapide, Câble de Charge USB-C Tressé en Nylon pour iPhone 16 15 Pro Max iPad Air Mini Samsung Galaxy S24 S23 S22 Ultra Xiaomi</t>
+          <t>UGREEN USB 3.0 Lecteur de Carte SD Micro Adaptateur 5Gbps Transfert Rapide Accès Simultané à 2 Cartes Max 2To Card Reader Supporter TF SDXC SDHC MMC pour Windows MacOS Linux</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>9,98</t>
+          <t>11,89</t>
         </is>
       </c>
     </row>
@@ -1869,12 +1869,12 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>CSL-Computer - Tapis de souris XXL Speed Gaming Titanwolf noir 900 x 400 mm - Grande base de table - Améliore la précision et la vitesse, 23032532, Type 1</t>
+          <t>Module de Refroidissement Thermoélectrique, Dissipateur de Chaleur Diamètre Extérieur 26 Mm TES1 04903 Électronique Circulaire Accessoires pour Ordinateur Composants Ventilateurs</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>12,95</t>
+          <t>12,18</t>
         </is>
       </c>
     </row>
@@ -1884,12 +1884,12 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Module de Refroidissement Thermoélectrique, Dissipateur de Chaleur Diamètre Extérieur 26 Mm TES1 04903 Électronique Circulaire Accessoires pour Ordinateur Composants Ventilateurs</t>
+          <t>Mikikit 1 Jeu Ordinateur M. 2 De Montage Composants De Montage Du Disque Dur Ssd Ssd Accessoire Informatique Pour M.2 Ssd Adaptateur Serveur Acier Inoxydable M2</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>18,06</t>
+          <t>17,28</t>
         </is>
       </c>
     </row>
@@ -1899,27 +1899,12 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Denash Carte PCI Carte Graphique VGA 8 Mo 32 Bits Ordinateur de Bureau Composants Accessoires Multi-Affichage pour ATI Rage XL</t>
+          <t>UKCOCO Accessoires Pour Ordinateur Portable D'Ordinateur 1 Pièce Composant De Bandoulière Matériel De Sport Pour Hommes Et Femmes Bretelles Réglables</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>19,42</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="n">
-        <v>99</v>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>UKCOCO Accessoires Pour Ordinateur Portable D'Ordinateur 1 Pièce Composant De Bandoulière Matériel De Sport Pour Hommes Et Femmes Bretelles Réglables</t>
-        </is>
-      </c>
-      <c r="C100" t="inlineStr">
-        <is>
-          <t>8,79</t>
+          <t>4,79</t>
         </is>
       </c>
     </row>

</xml_diff>